<commit_message>
indique les cargos basiques en bleu
</commit_message>
<xml_diff>
--- a/cargos/cargosList.xlsx
+++ b/cargos/cargosList.xlsx
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +205,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Fira Code Retina"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Fira Code Retina"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -277,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -288,12 +300,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -591,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:BF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,16 +933,16 @@
       <c r="B11" s="5">
         <v>6000</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -968,10 +987,10 @@
       <c r="AB11" t="s">
         <v>29</v>
       </c>
-      <c r="AD11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE11" t="s">
+      <c r="AD11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="AG11" s="4" t="s">
@@ -986,40 +1005,40 @@
       <c r="AK11" t="s">
         <v>29</v>
       </c>
-      <c r="AM11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AS11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AV11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AZ11" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="BC11" t="s">
+      <c r="AM11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AW11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="BC11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="BE11" s="4" t="s">
@@ -1045,10 +1064,10 @@
       <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="L12" s="4" t="s">
@@ -1057,28 +1076,28 @@
       <c r="M12" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P12" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" s="4" t="s">
+      <c r="O12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="U12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="V12" t="s">
-        <v>6</v>
-      </c>
-      <c r="X12" s="4" t="s">
+      <c r="U12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="X12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Y12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AA12" s="4" t="s">
@@ -1087,22 +1106,22 @@
       <c r="AB12" t="s">
         <v>40</v>
       </c>
-      <c r="AD12" s="4" t="s">
+      <c r="AD12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AG12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK12" t="s">
+      <c r="AG12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="AM12" s="4" t="s">
@@ -1141,10 +1160,10 @@
       <c r="BC12" t="s">
         <v>52</v>
       </c>
-      <c r="BE12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="BF12" t="s">
+      <c r="BE12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="BF12" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1153,10 +1172,10 @@
         <v>14000</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1185,10 +1204,10 @@
       <c r="Y13" t="s">
         <v>30</v>
       </c>
-      <c r="AA13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB13" t="s">
+      <c r="AA13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="AD13" s="4" t="s">
@@ -1260,17 +1279,17 @@
         <v>31</v>
       </c>
       <c r="R14" s="4"/>
-      <c r="U14" s="4" t="s">
+      <c r="U14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="X14" s="4"/>
-      <c r="AA14" s="4" t="s">
+      <c r="AA14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AB14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AD14" s="4" t="s">
@@ -1279,10 +1298,10 @@
       <c r="AE14" t="s">
         <v>43</v>
       </c>
-      <c r="AG14" s="4" t="s">
+      <c r="AG14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AH14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AJ14" s="4" t="s">
@@ -1298,10 +1317,10 @@
       <c r="AZ14" t="s">
         <v>31</v>
       </c>
-      <c r="BE14" s="4" t="s">
+      <c r="BE14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="BF14" t="s">
+      <c r="BF14" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1311,17 +1330,17 @@
       </c>
       <c r="C15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="11" t="s">
         <v>10</v>
       </c>
       <c r="R15" s="4"/>
@@ -1350,10 +1369,10 @@
       <c r="AH15" t="s">
         <v>30</v>
       </c>
-      <c r="AJ15" s="4" t="s">
+      <c r="AJ15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AK15" t="s">
+      <c r="AK15" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AM15" s="4"/>

</xml_diff>

<commit_message>
cargo : update "AXIS steel city"
</commit_message>
<xml_diff>
--- a/cargos/cargosList.xlsx
+++ b/cargos/cargosList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="95">
   <si>
     <t>Base game</t>
   </si>
@@ -187,13 +187,127 @@
   </si>
   <si>
     <t>Tourists</t>
+  </si>
+  <si>
+    <t>SALT</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>scrap metal</t>
+  </si>
+  <si>
+    <t>iron ore</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>oxygen</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>recycle</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>engineer suppl</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>bauxite</t>
+  </si>
+  <si>
+    <t>produce</t>
+  </si>
+  <si>
+    <t>limestone</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>pyrite ore</t>
+  </si>
+  <si>
+    <t>soda ash</t>
+  </si>
+  <si>
+    <t>tar</t>
+  </si>
+  <si>
+    <t>fish &amp; meat</t>
+  </si>
+  <si>
+    <t>metal parts</t>
+  </si>
+  <si>
+    <t>SCMT</t>
+  </si>
+  <si>
+    <t>SASH</t>
+  </si>
+  <si>
+    <t>SAND</t>
+  </si>
+  <si>
+    <t>RCYC</t>
+  </si>
+  <si>
+    <t>OIL_</t>
+  </si>
+  <si>
+    <t>LVST</t>
+  </si>
+  <si>
+    <t>IORE</t>
+  </si>
+  <si>
+    <t>GRAI</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>ENSP</t>
+  </si>
+  <si>
+    <t>AORE</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>PORE</t>
+  </si>
+  <si>
+    <t>O2__</t>
+  </si>
+  <si>
+    <t>CTAR</t>
+  </si>
+  <si>
+    <t>COAL</t>
+  </si>
+  <si>
+    <t>LIME</t>
+  </si>
+  <si>
+    <t>STSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +318,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Fira Code Retina"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Fira Code Retina"/>
     </font>
   </fonts>
@@ -277,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -288,6 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +710,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:BF18"/>
+  <dimension ref="B4:BF44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q12" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="AH29" sqref="AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,61 +906,61 @@
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AM8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AS8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AV8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AY8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BB8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE8" s="4" t="s">
+      <c r="C8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE8" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -843,61 +968,61 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AS9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AV9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AY9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="BB9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="BE9" s="4" t="s">
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AY9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BB9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE9" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1273,7 +1398,7 @@
       <c r="AB14" t="s">
         <v>10</v>
       </c>
-      <c r="AD14" s="4" t="s">
+      <c r="AD14" s="10" t="s">
         <v>14</v>
       </c>
       <c r="AE14" t="s">
@@ -1416,6 +1541,165 @@
       </c>
       <c r="BF18" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+    </row>
+    <row r="23" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD26" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD29" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD30" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:58" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD33" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD35" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD36" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD38" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD39" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="30:31" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="AD40" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD44" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>